<commit_message>
Ranking logic and a host of other changes.
</commit_message>
<xml_diff>
--- a/data/residents/test_scores.xlsx
+++ b/data/residents/test_scores.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="44">
   <si>
     <t xml:space="preserve">Table B1. Test Scores and Experiences of First-Year Residents, by Specialty</t>
   </si>
@@ -211,38 +211,6 @@
   </si>
   <si>
     <t xml:space="preserve">Vascular Surgery: Integrated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. All PGY1s in Pediatrics and in Obstetrics and Gynecology are included in the table above, including those for whom the position is a preliminary year for another specialty. Preliminary positions were not reported separately because they make up less than 3% of the first-year positions in each of these specialties.   </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Note:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Test score statistics with a total population fewer than 10 have been excluded, including specialties with fewer than 10 residents. More information on USMLE scores can be found at usmle.org/. More information on COMLEX scores can be found at nbome.org/exams-assessments/comlex-usa/.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Source: GME Track® as of Aug. 13, 2020; NBME as of Sept. 21, 2020; NBOME as of Aug. 14, 2020; ERAS as of July 6, 2020.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">© 2020 Association of American Medical Colleges. May be reproduced and distributed with attribution for educational and noncommercial purposes only.</t>
   </si>
 </sst>
 </file>
@@ -416,7 +384,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -428,7 +396,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -444,55 +412,55 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="2" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -590,9 +558,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>702360</xdr:colOff>
+      <xdr:colOff>701640</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>56520</xdr:rowOff>
+      <xdr:rowOff>56160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -605,8 +573,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12375000" y="22320"/>
-          <a:ext cx="507600" cy="386280"/>
+          <a:off x="13709880" y="22320"/>
+          <a:ext cx="506880" cy="385920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -678,17 +646,17 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="9" topLeftCell="B88" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="9" topLeftCell="B168" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B90" activeCellId="0" sqref="B90"/>
+      <selection pane="bottomLeft" activeCell="A189" activeCellId="0" sqref="A189"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.2890625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.28125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="36.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="46.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="7.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="8.7"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="10.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="10.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.43"/>
@@ -2116,7 +2084,7 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="18" t="s">
+      <c r="A47" s="19" t="s">
         <v>25</v>
       </c>
       <c r="B47" s="14" t="s">
@@ -2148,7 +2116,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="18" t="s">
+      <c r="A48" s="19" t="s">
         <v>25</v>
       </c>
       <c r="B48" s="14" t="s">
@@ -2340,7 +2308,7 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="20" t="s">
+      <c r="A54" s="21" t="s">
         <v>26</v>
       </c>
       <c r="B54" s="10" t="s">
@@ -2372,7 +2340,7 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="20" t="s">
+      <c r="A55" s="21" t="s">
         <v>26</v>
       </c>
       <c r="B55" s="10" t="s">
@@ -2404,7 +2372,7 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="20" t="s">
+      <c r="A56" s="21" t="s">
         <v>26</v>
       </c>
       <c r="B56" s="10" t="s">
@@ -2436,7 +2404,7 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="20" t="s">
+      <c r="A57" s="21" t="s">
         <v>26</v>
       </c>
       <c r="B57" s="10" t="s">
@@ -2468,7 +2436,7 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="20" t="s">
+      <c r="A58" s="21" t="s">
         <v>26</v>
       </c>
       <c r="B58" s="10" t="s">
@@ -2500,7 +2468,7 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="20" t="s">
+      <c r="A59" s="21" t="s">
         <v>26</v>
       </c>
       <c r="B59" s="10" t="s">
@@ -2532,7 +2500,7 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="20" t="s">
+      <c r="A60" s="21" t="s">
         <v>26</v>
       </c>
       <c r="B60" s="10" t="s">
@@ -3076,7 +3044,7 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="21" t="s">
+      <c r="A77" s="20" t="s">
         <v>30</v>
       </c>
       <c r="B77" s="14" t="s">
@@ -3108,7 +3076,7 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="21" t="s">
+      <c r="A78" s="20" t="s">
         <v>30</v>
       </c>
       <c r="B78" s="14" t="s">
@@ -3140,7 +3108,7 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="21" t="s">
+      <c r="A79" s="20" t="s">
         <v>30</v>
       </c>
       <c r="B79" s="14" t="s">
@@ -3172,7 +3140,7 @@
       </c>
     </row>
     <row r="80" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="21" t="s">
+      <c r="A80" s="20" t="s">
         <v>30</v>
       </c>
       <c r="B80" s="14" t="s">
@@ -3204,7 +3172,7 @@
       </c>
     </row>
     <row r="81" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="21" t="s">
+      <c r="A81" s="20" t="s">
         <v>30</v>
       </c>
       <c r="B81" s="14" t="s">
@@ -3236,7 +3204,7 @@
       </c>
     </row>
     <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="21" t="s">
+      <c r="A82" s="20" t="s">
         <v>30</v>
       </c>
       <c r="B82" s="14" t="s">
@@ -3268,7 +3236,7 @@
       </c>
     </row>
     <row r="83" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="21" t="s">
+      <c r="A83" s="20" t="s">
         <v>30</v>
       </c>
       <c r="B83" s="14" t="s">
@@ -3300,7 +3268,7 @@
       </c>
     </row>
     <row r="84" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="21" t="s">
+      <c r="A84" s="20" t="s">
         <v>30</v>
       </c>
       <c r="B84" s="14" t="s">
@@ -3588,7 +3556,7 @@
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A93" s="21" t="s">
+      <c r="A93" s="20" t="s">
         <v>32</v>
       </c>
       <c r="B93" s="14" t="s">
@@ -3620,7 +3588,7 @@
       </c>
     </row>
     <row r="94" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="21" t="s">
+      <c r="A94" s="20" t="s">
         <v>32</v>
       </c>
       <c r="B94" s="14" t="s">
@@ -3652,7 +3620,7 @@
       </c>
     </row>
     <row r="95" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="21" t="s">
+      <c r="A95" s="20" t="s">
         <v>32</v>
       </c>
       <c r="B95" s="14" t="s">
@@ -3684,7 +3652,7 @@
       </c>
     </row>
     <row r="96" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="21" t="s">
+      <c r="A96" s="20" t="s">
         <v>32</v>
       </c>
       <c r="B96" s="14" t="s">
@@ -3716,7 +3684,7 @@
       </c>
     </row>
     <row r="97" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="21" t="s">
+      <c r="A97" s="20" t="s">
         <v>32</v>
       </c>
       <c r="B97" s="14" t="s">
@@ -3748,7 +3716,7 @@
       </c>
     </row>
     <row r="98" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="21" t="s">
+      <c r="A98" s="20" t="s">
         <v>32</v>
       </c>
       <c r="B98" s="14" t="s">
@@ -3780,7 +3748,7 @@
       </c>
     </row>
     <row r="99" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="21" t="s">
+      <c r="A99" s="20" t="s">
         <v>32</v>
       </c>
       <c r="B99" s="14" t="s">
@@ -3812,7 +3780,7 @@
       </c>
     </row>
     <row r="100" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="21" t="s">
+      <c r="A100" s="20" t="s">
         <v>32</v>
       </c>
       <c r="B100" s="14" t="s">
@@ -4100,7 +4068,7 @@
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A109" s="21" t="s">
+      <c r="A109" s="20" t="s">
         <v>34</v>
       </c>
       <c r="B109" s="14" t="s">
@@ -4132,7 +4100,7 @@
       </c>
     </row>
     <row r="110" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="21" t="s">
+      <c r="A110" s="20" t="s">
         <v>34</v>
       </c>
       <c r="B110" s="14" t="s">
@@ -4164,7 +4132,7 @@
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A111" s="21" t="s">
+      <c r="A111" s="20" t="s">
         <v>34</v>
       </c>
       <c r="B111" s="14" t="s">
@@ -4196,7 +4164,7 @@
       </c>
     </row>
     <row r="112" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="21" t="s">
+      <c r="A112" s="20" t="s">
         <v>34</v>
       </c>
       <c r="B112" s="14" t="s">
@@ -4228,7 +4196,7 @@
       </c>
     </row>
     <row r="113" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="21" t="s">
+      <c r="A113" s="20" t="s">
         <v>34</v>
       </c>
       <c r="B113" s="14" t="s">
@@ -4260,7 +4228,7 @@
       </c>
     </row>
     <row r="114" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="21" t="s">
+      <c r="A114" s="20" t="s">
         <v>34</v>
       </c>
       <c r="B114" s="14" t="s">
@@ -4292,7 +4260,7 @@
       </c>
     </row>
     <row r="115" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="21" t="s">
+      <c r="A115" s="20" t="s">
         <v>34</v>
       </c>
       <c r="B115" s="14" t="s">
@@ -4324,7 +4292,7 @@
       </c>
     </row>
     <row r="116" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="21" t="s">
+      <c r="A116" s="20" t="s">
         <v>34</v>
       </c>
       <c r="B116" s="14" t="s">
@@ -4612,7 +4580,7 @@
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A125" s="21" t="s">
+      <c r="A125" s="20" t="s">
         <v>36</v>
       </c>
       <c r="B125" s="14" t="s">
@@ -4644,7 +4612,7 @@
       </c>
     </row>
     <row r="126" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="21" t="s">
+      <c r="A126" s="20" t="s">
         <v>36</v>
       </c>
       <c r="B126" s="14" t="s">
@@ -4676,7 +4644,7 @@
       </c>
     </row>
     <row r="127" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="21" t="s">
+      <c r="A127" s="20" t="s">
         <v>36</v>
       </c>
       <c r="B127" s="14" t="s">
@@ -4708,7 +4676,7 @@
       </c>
     </row>
     <row r="128" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="21" t="s">
+      <c r="A128" s="20" t="s">
         <v>36</v>
       </c>
       <c r="B128" s="14" t="s">
@@ -4740,7 +4708,7 @@
       </c>
     </row>
     <row r="129" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="21" t="s">
+      <c r="A129" s="20" t="s">
         <v>36</v>
       </c>
       <c r="B129" s="14" t="s">
@@ -4772,7 +4740,7 @@
       </c>
     </row>
     <row r="130" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="21" t="s">
+      <c r="A130" s="20" t="s">
         <v>36</v>
       </c>
       <c r="B130" s="14" t="s">
@@ -4804,7 +4772,7 @@
       </c>
     </row>
     <row r="131" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="21" t="s">
+      <c r="A131" s="20" t="s">
         <v>36</v>
       </c>
       <c r="B131" s="14" t="s">
@@ -4836,7 +4804,7 @@
       </c>
     </row>
     <row r="132" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="21" t="s">
+      <c r="A132" s="20" t="s">
         <v>36</v>
       </c>
       <c r="B132" s="14" t="s">
@@ -4868,7 +4836,7 @@
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A133" s="20" t="s">
+      <c r="A133" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B133" s="10" t="s">
@@ -4900,7 +4868,7 @@
       </c>
     </row>
     <row r="134" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A134" s="20" t="s">
+      <c r="A134" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B134" s="10" t="s">
@@ -4932,7 +4900,7 @@
       </c>
     </row>
     <row r="135" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="20" t="s">
+      <c r="A135" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B135" s="10" t="s">
@@ -4964,7 +4932,7 @@
       </c>
     </row>
     <row r="136" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="20" t="s">
+      <c r="A136" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B136" s="10" t="s">
@@ -4996,7 +4964,7 @@
       </c>
     </row>
     <row r="137" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="20" t="s">
+      <c r="A137" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B137" s="10" t="s">
@@ -5028,7 +4996,7 @@
       </c>
     </row>
     <row r="138" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="20" t="s">
+      <c r="A138" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B138" s="10" t="s">
@@ -5060,7 +5028,7 @@
       </c>
     </row>
     <row r="139" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="20" t="s">
+      <c r="A139" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B139" s="10" t="s">
@@ -5092,7 +5060,7 @@
       </c>
     </row>
     <row r="140" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="20" t="s">
+      <c r="A140" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B140" s="10" t="s">
@@ -5380,7 +5348,7 @@
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A149" s="20" t="s">
+      <c r="A149" s="21" t="s">
         <v>39</v>
       </c>
       <c r="B149" s="10" t="s">
@@ -5412,7 +5380,7 @@
       </c>
     </row>
     <row r="150" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="20" t="s">
+      <c r="A150" s="21" t="s">
         <v>39</v>
       </c>
       <c r="B150" s="10" t="s">
@@ -5444,7 +5412,7 @@
       </c>
     </row>
     <row r="151" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="20" t="s">
+      <c r="A151" s="21" t="s">
         <v>39</v>
       </c>
       <c r="B151" s="10" t="s">
@@ -5476,7 +5444,7 @@
       </c>
     </row>
     <row r="152" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="20" t="s">
+      <c r="A152" s="21" t="s">
         <v>39</v>
       </c>
       <c r="B152" s="10" t="s">
@@ -5508,7 +5476,7 @@
       </c>
     </row>
     <row r="153" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="20" t="s">
+      <c r="A153" s="21" t="s">
         <v>39</v>
       </c>
       <c r="B153" s="10" t="s">
@@ -5540,7 +5508,7 @@
       </c>
     </row>
     <row r="154" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="20" t="s">
+      <c r="A154" s="21" t="s">
         <v>39</v>
       </c>
       <c r="B154" s="10" t="s">
@@ -5572,7 +5540,7 @@
       </c>
     </row>
     <row r="155" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="20" t="s">
+      <c r="A155" s="21" t="s">
         <v>39</v>
       </c>
       <c r="B155" s="10" t="s">
@@ -5604,7 +5572,7 @@
       </c>
     </row>
     <row r="156" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="20" t="s">
+      <c r="A156" s="21" t="s">
         <v>39</v>
       </c>
       <c r="B156" s="10" t="s">
@@ -5636,7 +5604,7 @@
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A157" s="21" t="s">
+      <c r="A157" s="20" t="s">
         <v>40</v>
       </c>
       <c r="B157" s="14" t="s">
@@ -5668,7 +5636,7 @@
       </c>
     </row>
     <row r="158" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="21" t="s">
+      <c r="A158" s="20" t="s">
         <v>40</v>
       </c>
       <c r="B158" s="14" t="s">
@@ -5700,7 +5668,7 @@
       </c>
     </row>
     <row r="159" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="21" t="s">
+      <c r="A159" s="20" t="s">
         <v>40</v>
       </c>
       <c r="B159" s="14" t="s">
@@ -5732,7 +5700,7 @@
       </c>
     </row>
     <row r="160" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="21" t="s">
+      <c r="A160" s="20" t="s">
         <v>40</v>
       </c>
       <c r="B160" s="14" t="s">
@@ -5764,7 +5732,7 @@
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A161" s="21" t="s">
+      <c r="A161" s="20" t="s">
         <v>40</v>
       </c>
       <c r="B161" s="14" t="s">
@@ -5796,7 +5764,7 @@
       </c>
     </row>
     <row r="162" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="21" t="s">
+      <c r="A162" s="20" t="s">
         <v>40</v>
       </c>
       <c r="B162" s="14" t="s">
@@ -5828,7 +5796,7 @@
       </c>
     </row>
     <row r="163" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="21" t="s">
+      <c r="A163" s="20" t="s">
         <v>40</v>
       </c>
       <c r="B163" s="14" t="s">
@@ -5860,7 +5828,7 @@
       </c>
     </row>
     <row r="164" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="21" t="s">
+      <c r="A164" s="20" t="s">
         <v>40</v>
       </c>
       <c r="B164" s="14" t="s">
@@ -5892,7 +5860,7 @@
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A165" s="20" t="s">
+      <c r="A165" s="21" t="s">
         <v>41</v>
       </c>
       <c r="B165" s="10" t="s">
@@ -5924,7 +5892,7 @@
       </c>
     </row>
     <row r="166" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="20" t="s">
+      <c r="A166" s="21" t="s">
         <v>41</v>
       </c>
       <c r="B166" s="10" t="s">
@@ -5956,7 +5924,7 @@
       </c>
     </row>
     <row r="167" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="20" t="s">
+      <c r="A167" s="21" t="s">
         <v>41</v>
       </c>
       <c r="B167" s="10" t="s">
@@ -5988,7 +5956,7 @@
       </c>
     </row>
     <row r="168" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="20" t="s">
+      <c r="A168" s="21" t="s">
         <v>41</v>
       </c>
       <c r="B168" s="10" t="s">
@@ -6020,7 +5988,7 @@
       </c>
     </row>
     <row r="169" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="20" t="s">
+      <c r="A169" s="21" t="s">
         <v>41</v>
       </c>
       <c r="B169" s="10" t="s">
@@ -6052,7 +6020,7 @@
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A170" s="20" t="s">
+      <c r="A170" s="21" t="s">
         <v>41</v>
       </c>
       <c r="B170" s="10" t="s">
@@ -6084,7 +6052,7 @@
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A171" s="20" t="s">
+      <c r="A171" s="21" t="s">
         <v>41</v>
       </c>
       <c r="B171" s="10" t="s">
@@ -6116,7 +6084,7 @@
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A172" s="20" t="s">
+      <c r="A172" s="21" t="s">
         <v>41</v>
       </c>
       <c r="B172" s="10" t="s">
@@ -6660,9 +6628,7 @@
       </c>
     </row>
     <row r="189" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A189" s="19" t="s">
-        <v>44</v>
-      </c>
+      <c r="A189" s="19"/>
       <c r="B189" s="19"/>
       <c r="C189" s="19"/>
       <c r="D189" s="19"/>
@@ -6674,9 +6640,7 @@
       <c r="J189" s="19"/>
     </row>
     <row r="190" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A190" s="22" t="s">
-        <v>45</v>
-      </c>
+      <c r="A190" s="22"/>
       <c r="B190" s="22"/>
       <c r="C190" s="22"/>
       <c r="D190" s="22"/>
@@ -6687,10 +6651,8 @@
       <c r="I190" s="22"/>
       <c r="J190" s="22"/>
     </row>
-    <row r="191" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="23" t="s">
-        <v>46</v>
-      </c>
+    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="23"/>
       <c r="B191" s="23"/>
       <c r="C191" s="23"/>
       <c r="D191" s="23"/>
@@ -6701,10 +6663,8 @@
       <c r="I191" s="23"/>
       <c r="J191" s="23"/>
     </row>
-    <row r="192" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="24" t="s">
-        <v>47</v>
-      </c>
+    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="24"/>
       <c r="B192" s="24"/>
       <c r="C192" s="24"/>
       <c r="D192" s="24"/>
@@ -6724,7 +6684,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="40">
+  <mergeCells count="31">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A3:A4"/>
@@ -6753,15 +6713,6 @@
     <mergeCell ref="A50:A51"/>
     <mergeCell ref="A51:A52"/>
     <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A181:A182"/>
-    <mergeCell ref="A182:A183"/>
-    <mergeCell ref="A183:A184"/>
-    <mergeCell ref="A184:A185"/>
-    <mergeCell ref="A185:A186"/>
-    <mergeCell ref="A186:A187"/>
-    <mergeCell ref="A187:A188"/>
-    <mergeCell ref="A188:A189"/>
-    <mergeCell ref="A189:J189"/>
     <mergeCell ref="A190:J190"/>
     <mergeCell ref="A191:J191"/>
     <mergeCell ref="A192:J192"/>

</xml_diff>